<commit_message>
Changed PoE module to accomodate USB_VBUS, changed Rectifiers, added level shifter
</commit_message>
<xml_diff>
--- a/Hardware/v2/PoE BOM.xlsx
+++ b/Hardware/v2/PoE BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>http://www.silvertel.com/images/datasheets/Ag9800M-datasheet-miniature-isolated-Power-over-Ethernet-PoE-module-solution.pdf</t>
   </si>
@@ -84,12 +84,6 @@
     <t>Bridge Rectifier</t>
   </si>
   <si>
-    <t>http://www.vishay.com/docs/88661/mb2s.pdf</t>
-  </si>
-  <si>
-    <t>MB4S-E3/45</t>
-  </si>
-  <si>
     <t>CAP-10300</t>
   </si>
   <si>
@@ -121,6 +115,66 @@
   </si>
   <si>
     <t>F12CAP</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/DF1510S-E3%2F77/DF1510S-E3%2F77GICT-ND/3711737</t>
+  </si>
+  <si>
+    <t>DF1510S</t>
+  </si>
+  <si>
+    <t>http://www.vishay.com/docs/88570/df15005s.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/tps62065.pdf</t>
+  </si>
+  <si>
+    <t>TPS62065</t>
+  </si>
+  <si>
+    <t>Capacitor (22uF)</t>
+  </si>
+  <si>
+    <t>CAP-08402</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/CL21A226MQCLQNC/1276-2412-1-ND/3890498</t>
+  </si>
+  <si>
+    <t>Capacitor (47pF)</t>
+  </si>
+  <si>
+    <t>CAP-08913</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/CL10C470JB8NNNC/1276-1037-1-ND/3889123</t>
+  </si>
+  <si>
+    <t>Resistor (680K)</t>
+  </si>
+  <si>
+    <t>RESISTOR0402 (RESISTOR)</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RC0402JR-07680KL/311-680KJRCT-ND/729448</t>
+  </si>
+  <si>
+    <t>Resistor (120K)</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RC0402JR-07120KL/311-120KJRCT-ND/729368</t>
+  </si>
+  <si>
+    <t>Inductor (1uH)</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/BRL3225T1R0M/587-2164-1-ND/2002862</t>
+  </si>
+  <si>
+    <t>INDUCTOR 1210 (INDUCTOR)</t>
+  </si>
+  <si>
+    <t>Eagle Code</t>
   </si>
 </sst>
 </file>
@@ -470,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G15"/>
+  <dimension ref="B3:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,16 +535,19 @@
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
@@ -498,7 +555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -512,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -526,7 +583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>19</v>
       </c>
@@ -537,7 +594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>18</v>
       </c>
@@ -548,115 +605,212 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>22</v>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1"/>
     <hyperlink ref="G10" r:id="rId2"/>
-    <hyperlink ref="G15" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tied DCIN to VSYS, added LED, cleaned up Bridge Rectifiers
</commit_message>
<xml_diff>
--- a/Hardware/v2/PoE BOM.xlsx
+++ b/Hardware/v2/PoE BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>http://www.silvertel.com/images/datasheets/Ag9800M-datasheet-miniature-isolated-Power-over-Ethernet-PoE-module-solution.pdf</t>
   </si>
@@ -75,12 +75,6 @@
     <t>Capacitor (.1uF)</t>
   </si>
   <si>
-    <t>Resistor (0ohm)</t>
-  </si>
-  <si>
-    <t>R-US_R1210</t>
-  </si>
-  <si>
     <t>Bridge Rectifier</t>
   </si>
   <si>
@@ -135,12 +129,6 @@
     <t>Capacitor (22uF)</t>
   </si>
   <si>
-    <t>CAP-08402</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/CL21A226MQCLQNC/1276-2412-1-ND/3890498</t>
-  </si>
-  <si>
     <t>Capacitor (47pF)</t>
   </si>
   <si>
@@ -168,13 +156,49 @@
     <t>Inductor (1uH)</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/BRL3225T1R0M/587-2164-1-ND/2002862</t>
-  </si>
-  <si>
     <t>INDUCTOR 1210 (INDUCTOR)</t>
   </si>
   <si>
     <t>Eagle Code</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/LQM32PN1R0MG0L/490-10767-1-ND/5251332</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/GRM188R60G226MEA0D/490-5526-1-ND/2334922</t>
+  </si>
+  <si>
+    <t>GRM188R60G226MEA0D</t>
+  </si>
+  <si>
+    <t>CL10C470JB8NNNC</t>
+  </si>
+  <si>
+    <t>LQM32PN1R0MG0L</t>
+  </si>
+  <si>
+    <t>Resistor (1K)</t>
+  </si>
+  <si>
+    <t>RES-07856</t>
+  </si>
+  <si>
+    <t>RC0603JR-071KL</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RC0603JR-071KL/311-1.0KGRCT-ND/729624</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>DIO-08575</t>
+  </si>
+  <si>
+    <t>LTST-C191TBKT</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/LTST-C191TBKT/160-1647-1-ND/573587</t>
   </si>
 </sst>
 </file>
@@ -524,17 +548,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G24"/>
+  <dimension ref="B3:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -546,7 +570,7 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -585,10 +609,10 @@
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -596,125 +620,137 @@
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="F7">
         <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>30</v>
+      <c r="G8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
         <v>41</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -725,94 +761,112 @@
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G18" s="1"/>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
       </c>
       <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
       </c>
       <c r="F22">
         <v>2</v>
       </c>
+      <c r="G22" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G24" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1"/>
-    <hyperlink ref="G10" r:id="rId2"/>
+    <hyperlink ref="G9" r:id="rId2"/>
+    <hyperlink ref="G15" r:id="rId3"/>
+    <hyperlink ref="G11" r:id="rId4"/>
+    <hyperlink ref="G12" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added R for min load
</commit_message>
<xml_diff>
--- a/Hardware/v2/PoE BOM.xlsx
+++ b/Hardware/v2/PoE BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>http://www.silvertel.com/images/datasheets/Ag9800M-datasheet-miniature-isolated-Power-over-Ethernet-PoE-module-solution.pdf</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/LTST-C191TBKT/160-1647-1-ND/573587</t>
+  </si>
+  <si>
+    <t>Resistor (25)</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/504L25R0FTNCFT/1284-1325-1-ND/4789905</t>
+  </si>
+  <si>
+    <t>504L25R0FTNCFT</t>
+  </si>
+  <si>
+    <t>R-US_R0402</t>
   </si>
 </sst>
 </file>
@@ -548,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G23"/>
+  <dimension ref="B3:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,67 +805,84 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>17</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>11</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F22">
         <v>2</v>
       </c>
-      <c r="G22" s="1" t="s">
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G23" t="s">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added downstream USB through hirose, fixed some connections between top and bottom connectors
</commit_message>
<xml_diff>
--- a/Hardware/v2/PoE BOM.xlsx
+++ b/Hardware/v2/PoE BOM.xlsx
@@ -563,7 +563,7 @@
   <dimension ref="B3:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,7 +703,7 @@
         <v>38</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
PoE Board completed. Added Micro USB to schematic and board
</commit_message>
<xml_diff>
--- a/Hardware/v2/PoE BOM.xlsx
+++ b/Hardware/v2/PoE BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="119">
   <si>
     <t>http://www.silvertel.com/images/datasheets/Ag9800M-datasheet-miniature-isolated-Power-over-Ethernet-PoE-module-solution.pdf</t>
   </si>
@@ -189,9 +189,6 @@
     <t>http://www.digikey.com/product-detail/en/RC0603JR-071KL/311-1.0KGRCT-ND/729624</t>
   </si>
   <si>
-    <t>LED</t>
-  </si>
-  <si>
     <t>DIO-08575</t>
   </si>
   <si>
@@ -201,16 +198,181 @@
     <t>http://www.digikey.com/product-detail/en/LTST-C191TBKT/160-1647-1-ND/573587</t>
   </si>
   <si>
-    <t>Resistor (25)</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/504L25R0FTNCFT/1284-1325-1-ND/4789905</t>
-  </si>
-  <si>
-    <t>504L25R0FTNCFT</t>
-  </si>
-  <si>
     <t>R-US_R0402</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/0402zd104kat2a/ceramic-capacitor-0-1uf-10v-x5r/dp/96M1117?ost=96M1117</t>
+  </si>
+  <si>
+    <t>C30</t>
+  </si>
+  <si>
+    <t>C35</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>C32</t>
+  </si>
+  <si>
+    <t>C31</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>C29, C28</t>
+  </si>
+  <si>
+    <t>B1, B2</t>
+  </si>
+  <si>
+    <t>Resistor (0)</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/vishay-dale/crcw12100000z0ea/resistor-chip-jumper-zero-ohm/dp/72M6870?ost=72M6870</t>
+  </si>
+  <si>
+    <t>C33, C34</t>
+  </si>
+  <si>
+    <t>USB Micro B stuff</t>
+  </si>
+  <si>
+    <t>http://cdn.sparkfun.com/datasheets/Components/General%20IC/DS_FT231X.pdf</t>
+  </si>
+  <si>
+    <t>FT231XS</t>
+  </si>
+  <si>
+    <t>FTDI chip</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>Micro USB</t>
+  </si>
+  <si>
+    <t>SSOP20_L</t>
+  </si>
+  <si>
+    <t>USB-B-MICRO-SMD-V03</t>
+  </si>
+  <si>
+    <t>C36, C37</t>
+  </si>
+  <si>
+    <t>C38, C39</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/ERJ-2RKF27R0X/P27.0LCT-ND/1746665</t>
+  </si>
+  <si>
+    <t>Resistor (27)</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF27R0X</t>
+  </si>
+  <si>
+    <t>R22, R23</t>
+  </si>
+  <si>
+    <t>R24, R25</t>
+  </si>
+  <si>
+    <t>Resistor (100)</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1000X</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/ERJ-2RKF1000X/P100LCT-ND/194126</t>
+  </si>
+  <si>
+    <t>R26, R27</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/ERJ-2RKF1001X/P1.00KLCT-ND/97341</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1001X</t>
+  </si>
+  <si>
+    <t>LED (Blue)</t>
+  </si>
+  <si>
+    <t>LED (Yellow)</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/LTST-C191KSKT/160-1448-1-ND/386838</t>
+  </si>
+  <si>
+    <t>LTST-C191KSKT</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>LED (Red)</t>
+  </si>
+  <si>
+    <t>LTST-C191KRKT</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/LTST-C191KRKT/160-1447-1-ND/386836</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>DIO-00819</t>
+  </si>
+  <si>
+    <t>DIO-09003</t>
+  </si>
+  <si>
+    <t>R21, R28</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/PHP01206E20R0BST5/PHP20.0ACT-ND/2508155</t>
+  </si>
+  <si>
+    <t>Resistor (20) (1W)</t>
+  </si>
+  <si>
+    <t>PHP01206E20R0BST5</t>
   </si>
 </sst>
 </file>
@@ -242,11 +404,20 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -255,9 +426,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -560,21 +733,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G24"/>
+  <dimension ref="A3:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>3</v>
       </c>
@@ -591,7 +764,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -605,7 +781,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -619,7 +798,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
@@ -629,8 +814,17 @@
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="G6" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
@@ -647,7 +841,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
@@ -661,7 +861,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
@@ -678,7 +884,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -692,7 +904,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>81</v>
+      </c>
       <c r="C11" t="s">
         <v>36</v>
       </c>
@@ -703,13 +921,19 @@
         <v>38</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
       <c r="C12" t="s">
         <v>37</v>
       </c>
@@ -726,7 +950,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
       <c r="C13" t="s">
         <v>40</v>
       </c>
@@ -740,7 +970,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
       <c r="C14" t="s">
         <v>43</v>
       </c>
@@ -754,7 +990,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
       <c r="C15" t="s">
         <v>45</v>
       </c>
@@ -771,7 +1013,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
       <c r="C16" t="s">
         <v>53</v>
       </c>
@@ -788,102 +1036,358 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
       <c r="C17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
         <v>57</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23">
+      <c r="G33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34">
         <v>2</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G24" t="s">
-        <v>33</v>
+      <c r="G34" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" t="s">
+        <v>107</v>
+      </c>
+      <c r="E36" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" t="s">
+        <v>110</v>
+      </c>
+      <c r="E37" t="s">
+        <v>113</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -893,9 +1397,13 @@
     <hyperlink ref="G15" r:id="rId3"/>
     <hyperlink ref="G11" r:id="rId4"/>
     <hyperlink ref="G12" r:id="rId5"/>
+    <hyperlink ref="G6" r:id="rId6"/>
+    <hyperlink ref="G19" r:id="rId7"/>
+    <hyperlink ref="G32" r:id="rId8"/>
+    <hyperlink ref="G31" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed some stuff from DRC
</commit_message>
<xml_diff>
--- a/Hardware/v2/PoE BOM.xlsx
+++ b/Hardware/v2/PoE BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="120">
   <si>
     <t>http://www.silvertel.com/images/datasheets/Ag9800M-datasheet-miniature-isolated-Power-over-Ethernet-PoE-module-solution.pdf</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Level Shifter</t>
   </si>
   <si>
-    <t>TXB0108</t>
-  </si>
-  <si>
     <t>http://www.ti.com/lit/ds/symlink/txb0108.pdf</t>
   </si>
   <si>
@@ -373,6 +370,12 @@
   </si>
   <si>
     <t>PHP01206E20R0BST5</t>
+  </si>
+  <si>
+    <t>TXB0108 (SON)</t>
+  </si>
+  <si>
+    <t>UFDFN-20</t>
   </si>
 </sst>
 </file>
@@ -735,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,7 +758,7 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -766,7 +769,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -783,7 +786,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -800,317 +803,320 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
         <v>37</v>
       </c>
-      <c r="D12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
         <v>65</v>
       </c>
-      <c r="B13" t="s">
-        <v>66</v>
-      </c>
       <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
         <v>40</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
         <v>45</v>
       </c>
-      <c r="D15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" t="s">
-        <v>46</v>
-      </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" t="s">
         <v>53</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E16" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="E17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" t="s">
         <v>117</v>
       </c>
-      <c r="D18" t="s">
-        <v>118</v>
-      </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19">
         <v>2</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>9</v>
+      <c r="A22" t="s">
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -1124,36 +1130,39 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
       </c>
       <c r="D23" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24">
         <v>2</v>
@@ -1161,72 +1170,72 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F25">
         <v>2</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
         <v>87</v>
       </c>
-      <c r="C30" t="s">
-        <v>88</v>
-      </c>
       <c r="E30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1234,160 +1243,160 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31">
         <v>2</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" t="s">
         <v>37</v>
       </c>
-      <c r="D32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" t="s">
         <v>94</v>
       </c>
-      <c r="D33" t="s">
-        <v>95</v>
-      </c>
       <c r="E33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F33">
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" t="s">
         <v>97</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>98</v>
       </c>
-      <c r="D34" t="s">
-        <v>99</v>
-      </c>
       <c r="E34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F34">
         <v>2</v>
       </c>
       <c r="G34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F35">
         <v>2</v>
       </c>
       <c r="G35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
         <v>105</v>
-      </c>
-      <c r="D36" t="s">
-        <v>107</v>
-      </c>
-      <c r="E36" t="s">
-        <v>114</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" t="s">
         <v>112</v>
       </c>
-      <c r="C37" t="s">
-        <v>109</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
         <v>110</v>
-      </c>
-      <c r="E37" t="s">
-        <v>113</v>
-      </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1401,9 +1410,10 @@
     <hyperlink ref="G19" r:id="rId7"/>
     <hyperlink ref="G32" r:id="rId8"/>
     <hyperlink ref="G31" r:id="rId9"/>
+    <hyperlink ref="G23" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added ground fills. PoE: power planes around U7, diode for power through microB. Small: changed C26 to 2 caps, removed NP caps, removed test points, replaced crystal
</commit_message>
<xml_diff>
--- a/Hardware/v2/PoE BOM.xlsx
+++ b/Hardware/v2/PoE BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="125">
   <si>
     <t>http://www.silvertel.com/images/datasheets/Ag9800M-datasheet-miniature-isolated-Power-over-Ethernet-PoE-module-solution.pdf</t>
   </si>
@@ -376,6 +376,21 @@
   </si>
   <si>
     <t>UFDFN-20</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/VS-MBRA140TRPBF/VS-MBRA140TRPBFCT-ND/2687965</t>
+  </si>
+  <si>
+    <t>VS-MBRA140TRPBF</t>
+  </si>
+  <si>
+    <t>SMA-DIODE</t>
+  </si>
+  <si>
+    <t>D5</t>
   </si>
 </sst>
 </file>
@@ -736,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G37"/>
+  <dimension ref="A3:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1397,6 +1412,29 @@
       </c>
       <c r="G37" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" t="s">
+        <v>120</v>
+      </c>
+      <c r="D38" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" t="s">
+        <v>123</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed stub traces around Edison connector
</commit_message>
<xml_diff>
--- a/Hardware/v2/PoE BOM.xlsx
+++ b/Hardware/v2/PoE BOM.xlsx
@@ -1976,8 +1976,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="G43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2689,7 +2689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -4057,7 +4057,7 @@
       <c r="I49" t="s">
         <v>352</v>
       </c>
-      <c r="L49" t="s">
+      <c r="L49" s="3" t="s">
         <v>353</v>
       </c>
       <c r="M49">

</xml_diff>

<commit_message>
Added LDO for power off VSYS, fixed SD card
</commit_message>
<xml_diff>
--- a/Hardware/v2/PoE BOM.xlsx
+++ b/Hardware/v2/PoE BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="5832" windowWidth="23064" windowHeight="5832"/>
+    <workbookView xWindow="-432" yWindow="4404" windowWidth="22224" windowHeight="13896"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="376">
   <si>
     <t>Qty</t>
   </si>
@@ -1076,13 +1076,79 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/TPS62065DSGR/296-39441-1-ND/5143389</t>
+  </si>
+  <si>
+    <t>.1uF</t>
+  </si>
+  <si>
+    <t>0.1UF-16V(+-10%)(0402)</t>
+  </si>
+  <si>
+    <t>0402-CAP</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>C1005X5R1H104K050BB</t>
+  </si>
+  <si>
+    <t>445-5942-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/C1005X5R1H104K050BB/445-5942-1-ND/2443982</t>
+  </si>
+  <si>
+    <t>1.0UF-16V-10%(0402)</t>
+  </si>
+  <si>
+    <t>GRM155R60J105KE19D</t>
+  </si>
+  <si>
+    <t>490-1320-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/GRM155R60J105KE19D/490-1320-1-ND/587919</t>
+  </si>
+  <si>
+    <t>MIC5353-3.3YMT</t>
+  </si>
+  <si>
+    <t>MIC5353-XXYMT</t>
+  </si>
+  <si>
+    <t>6-UFDFN</t>
+  </si>
+  <si>
+    <t>IC REG LDO 3.3V 0.5A 6TMLF</t>
+  </si>
+  <si>
+    <t>Micrel</t>
+  </si>
+  <si>
+    <t>MIC5353-3.3YMT TR</t>
+  </si>
+  <si>
+    <t>576-3680-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/MIC5353-3.3YMT%20TR/576-3680-1-ND/2339682</t>
+  </si>
+  <si>
+    <t>C42, C43</t>
+  </si>
+  <si>
+    <t>C40, C41</t>
+  </si>
+  <si>
+    <t>U9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1241,6 +1307,26 @@
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1588,7 +1674,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1598,6 +1684,12 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="10" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1644,7 +1736,10 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1659,8 +1754,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="BOM" displayName="BOM" ref="A1:O51" totalsRowShown="0">
-  <autoFilter ref="A1:O51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="BOM" displayName="BOM" ref="A1:O54" totalsRowShown="0">
+  <autoFilter ref="A1:O54"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Qty"/>
     <tableColumn id="2" name="Value"/>
@@ -1675,11 +1770,11 @@
     <tableColumn id="10" name="Newark Part Number"/>
     <tableColumn id="13" name="URL"/>
     <tableColumn id="15" name="Price ea." dataCellStyle="Hyperlink"/>
-    <tableColumn id="12" name="Price ea. Order">
+    <tableColumn id="12" name="Price ea. Order" dataDxfId="0">
       <calculatedColumnFormula>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Final order qty" dataDxfId="0">
-      <calculatedColumnFormula>N53*BOM[[#This Row],[Qty]]</calculatedColumnFormula>
+    <tableColumn id="16" name="Final order qty" dataDxfId="1">
+      <calculatedColumnFormula>N56*BOM[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1974,10 +2069,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2083,7 +2178,7 @@
         <v>0.74399999999999999</v>
       </c>
       <c r="O2">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>15</v>
       </c>
     </row>
@@ -2126,7 +2221,7 @@
         <v>2E-3</v>
       </c>
       <c r="O3">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2169,7 +2264,7 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="O4">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2212,7 +2307,7 @@
         <v>0.126</v>
       </c>
       <c r="O5">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>105</v>
       </c>
     </row>
@@ -2255,7 +2350,7 @@
         <v>0.48</v>
       </c>
       <c r="O6">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -2298,7 +2393,7 @@
         <v>2E-3</v>
       </c>
       <c r="O7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2341,7 +2436,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="O8">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -2384,7 +2479,7 @@
         <v>1E-3</v>
       </c>
       <c r="O9">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2427,7 +2522,7 @@
         <v>3.1E-2</v>
       </c>
       <c r="O10">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2470,7 +2565,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="O11">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2513,7 +2608,7 @@
         <v>3.39</v>
       </c>
       <c r="O12">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2556,7 +2651,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="O13">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>20</v>
       </c>
     </row>
@@ -2599,7 +2694,7 @@
         <v>1E-3</v>
       </c>
       <c r="O14">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2642,7 +2737,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="O15">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -2685,7 +2780,7 @@
         <v>0.69099999999999995</v>
       </c>
       <c r="O16">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2728,7 +2823,7 @@
         <v>0.20100000000000001</v>
       </c>
       <c r="O17">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>15</v>
       </c>
     </row>
@@ -2771,7 +2866,7 @@
         <v>0.22</v>
       </c>
       <c r="O18">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -2814,7 +2909,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="O19">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2857,7 +2952,7 @@
         <v>0.26800000000000002</v>
       </c>
       <c r="O20">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>20</v>
       </c>
     </row>
@@ -2897,7 +2992,7 @@
         <v>1.44</v>
       </c>
       <c r="O21">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2940,7 +3035,7 @@
         <v>1.37</v>
       </c>
       <c r="O22">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2986,7 +3081,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="O23">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3023,7 +3118,7 @@
         <v>0.85</v>
       </c>
       <c r="O24">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3069,7 +3164,7 @@
         <v>4.72</v>
       </c>
       <c r="O25">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3112,7 +3207,7 @@
         <v>2.75</v>
       </c>
       <c r="O26">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3155,7 +3250,7 @@
         <v>0.69599999999999995</v>
       </c>
       <c r="O27">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
       <c r="P27" s="1"/>
@@ -3199,7 +3294,7 @@
         <v>2.63</v>
       </c>
       <c r="O28" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
       <c r="P28" s="1"/>
@@ -3240,7 +3335,7 @@
         <v>0.21</v>
       </c>
       <c r="O29" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
       <c r="P29" s="1"/>
@@ -3281,7 +3376,7 @@
         <v>0.76</v>
       </c>
       <c r="O30" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -3321,7 +3416,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="O31" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>15</v>
       </c>
     </row>
@@ -3364,7 +3459,7 @@
         <v>0.1</v>
       </c>
       <c r="O32" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3407,7 +3502,7 @@
         <v>0.1</v>
       </c>
       <c r="O33" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3450,7 +3545,7 @@
         <v>0.1</v>
       </c>
       <c r="O34" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3493,7 +3588,7 @@
         <v>3.53</v>
       </c>
       <c r="O35" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3536,7 +3631,7 @@
         <v>0.2</v>
       </c>
       <c r="O36" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -3579,7 +3674,7 @@
         <v>0.2</v>
       </c>
       <c r="O37" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -3622,7 +3717,7 @@
         <v>0.2</v>
       </c>
       <c r="O38" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -3665,7 +3760,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="O39" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3708,7 +3803,7 @@
         <v>0.46</v>
       </c>
       <c r="O40" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3751,7 +3846,7 @@
         <v>0.3</v>
       </c>
       <c r="O41" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3794,7 +3889,7 @@
         <v>0.32</v>
       </c>
       <c r="O42" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3837,7 +3932,7 @@
         <v>0.51</v>
       </c>
       <c r="O43" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3877,7 +3972,7 @@
         <v>0.43</v>
       </c>
       <c r="O44" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3920,7 +4015,7 @@
         <v>1.38</v>
       </c>
       <c r="O45" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -3954,7 +4049,7 @@
         <v>1.5</v>
       </c>
       <c r="O46" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -3988,7 +4083,7 @@
         <v>3.95</v>
       </c>
       <c r="O47" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -4028,11 +4123,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="O48">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1</v>
       </c>
@@ -4068,11 +4163,11 @@
         <v>2.44</v>
       </c>
       <c r="O49">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1</v>
       </c>
@@ -4108,72 +4203,202 @@
         <v>2.29</v>
       </c>
       <c r="O50" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>354</v>
+      </c>
+      <c r="C51" t="s">
+        <v>355</v>
+      </c>
+      <c r="D51" t="s">
+        <v>356</v>
+      </c>
+      <c r="E51" t="s">
+        <v>374</v>
+      </c>
+      <c r="F51" t="s">
+        <v>87</v>
+      </c>
+      <c r="G51" t="s">
+        <v>357</v>
+      </c>
+      <c r="H51" t="s">
+        <v>358</v>
+      </c>
+      <c r="I51" t="s">
+        <v>359</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="M51">
+        <v>0.13</v>
+      </c>
+      <c r="N51">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.26</v>
+      </c>
+      <c r="O51" s="7">
+        <f>N56*BOM[[#This Row],[Qty]]</f>
+        <v>10</v>
+      </c>
+      <c r="P51" s="1"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" t="s">
+        <v>361</v>
+      </c>
+      <c r="D52" t="s">
+        <v>356</v>
+      </c>
+      <c r="E52" t="s">
+        <v>373</v>
+      </c>
+      <c r="F52" t="s">
+        <v>87</v>
+      </c>
+      <c r="G52" t="s">
+        <v>116</v>
+      </c>
+      <c r="H52" t="s">
+        <v>362</v>
+      </c>
+      <c r="I52" t="s">
+        <v>363</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="M52" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="N52">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.2</v>
+      </c>
+      <c r="O52" s="7">
+        <f>N56*BOM[[#This Row],[Qty]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="9">
         <v>1</v>
       </c>
-      <c r="C51" t="s">
+      <c r="B53" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="L53" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="M53" s="9">
+        <v>0.91</v>
+      </c>
+      <c r="N53" s="9">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.91</v>
+      </c>
+      <c r="O53" s="11">
+        <f>N56*BOM[[#This Row],[Qty]]</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
         <v>198</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D54" t="s">
         <v>199</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E54" t="s">
         <v>198</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F54" t="s">
         <v>200</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G54" t="s">
         <v>201</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H54" t="s">
         <v>198</v>
       </c>
-      <c r="L51" s="3" t="s">
+      <c r="L54" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="M51">
+      <c r="M54">
         <v>7.76</v>
       </c>
-      <c r="N51">
+      <c r="N54">
         <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
         <v>7.76</v>
       </c>
-      <c r="O51" s="7">
-        <f>N53*BOM[[#This Row],[Qty]]</f>
+      <c r="O54" s="7">
+        <f>N56*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A52" s="2"/>
-      <c r="M52" s="5" t="s">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A55" s="2"/>
+      <c r="M55" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="N52" s="5">
+      <c r="N55" s="5">
         <f>SUM(BOM[Price ea. Order])</f>
-        <v>51.526000000000003</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M53" s="5" t="s">
+        <v>52.896000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M56" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="N53" s="5">
+      <c r="N56" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M54" s="6" t="s">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M57" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="N54" s="5">
-        <f>N52*N53</f>
-        <v>257.63</v>
+      <c r="N57" s="5">
+        <f>N55*N56</f>
+        <v>264.48</v>
       </c>
     </row>
   </sheetData>
@@ -4207,9 +4432,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId27"/>
-  <ignoredErrors>
-    <ignoredError sqref="N24" evalError="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId28"/>
   </tableParts>

</xml_diff>